<commit_message>
Fixed The Excel output bug & Form Validation for Registration and Login is finished
</commit_message>
<xml_diff>
--- a/src/test/api/template/template_excel.xlsx
+++ b/src/test/api/template/template_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickb\Documents\projects\gruenwerk-rapport-blatt-app\src\test\api\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43C4CB16-1188-4CED-BE43-AE6DA77BB225}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06368C9E-F093-4F1A-9BDB-136F382DCEAB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32768" yWindow="32768" windowWidth="19988" windowHeight="7980"/>
+    <workbookView xWindow="32768" yWindow="32768" windowWidth="19988" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verein" sheetId="1" r:id="rId1"/>
@@ -115,12 +115,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
-    <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="183" formatCode="dd/mm"/>
-    <numFmt numFmtId="184" formatCode="ddd"/>
-    <numFmt numFmtId="186" formatCode="mmmm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="mmmm"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -426,18 +423,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -465,38 +450,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="184" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="183" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -514,6 +474,15 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -523,23 +492,48 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_Stdblatt Verein" xfId="1"/>
+    <cellStyle name="Standard_Stdblatt Verein" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -942,12 +936,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="A9:F39"/>
+      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="12.4"/>
@@ -967,10 +961,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
@@ -981,28 +975,28 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="20" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="21"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="14.65">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="4"/>
@@ -1013,505 +1007,506 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="13.5">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="30" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="22" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="3.75" customHeight="1">
-      <c r="B6" s="26"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="48" t="s">
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="49"/>
-    </row>
-    <row r="8" spans="1:14" s="38" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A8" s="46" t="s">
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:14" s="28" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A20" s="27"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="27"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="27"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A31" s="27"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A32" s="27"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A33" s="27"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A35" s="27"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A37" s="27"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A38" s="27"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A39" s="27"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
     </row>
     <row r="40" spans="1:12" ht="8.25" customHeight="1">
       <c r="A40" s="3"/>
@@ -1531,23 +1526,23 @@
       <c r="C41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="8">
         <f>SUM(D9:D39)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="8">
         <f>SUM(E9:E39)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="8">
         <f>SUM(F9:F39)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="8">
         <f>SUM(G9:G39)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="8">
         <f>SUM(H9:H39)</f>
         <v>0</v>
       </c>
@@ -1572,23 +1567,23 @@
       <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="9">
         <f>SUM(D41*25)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="9">
         <f>SUM(E41*25)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="9">
         <f>SUM(F41*25)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="9">
         <f>SUM(G41*25)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="9">
         <f>SUM(H41*0)</f>
         <v>0</v>
       </c>
@@ -1610,14 +1605,14 @@
     <row r="45" spans="1:12">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="14">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="11">
         <f>SUM(D43:H43)</f>
         <v>0</v>
       </c>
@@ -1639,16 +1634,16 @@
     <row r="47" spans="1:12">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="15">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="12">
         <f>SUM(J9:J39)</f>
         <v>0</v>
       </c>
@@ -1668,16 +1663,16 @@
     <row r="49" spans="1:10">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="14">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1696,16 +1691,16 @@
     <row r="51" spans="1:10" ht="12.75" thickBot="1">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="42">
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="32">
         <f>H45+J47+J49</f>
         <v>0</v>
       </c>
@@ -1722,32 +1717,16 @@
     <row r="54" spans="1:10">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="41"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="D7:H7"/>
@@ -1758,12 +1737,28 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E4:G4"/>
     <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K34:L34"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.24" right="0.15748031496062992" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0"/>

</xml_diff>